<commit_message>
add full text search to sql script & table design
</commit_message>
<xml_diff>
--- a/doc/detail_design/db/MiniBlog_Database_Design.xlsx
+++ b/doc/detail_design/db/MiniBlog_Database_Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27200" windowHeight="17040" tabRatio="818" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27200" windowHeight="17040" tabRatio="818" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="246">
   <si>
     <t>No</t>
   </si>
@@ -904,6 +904,42 @@
   </si>
   <si>
     <t>updated_dt</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>username</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>username, firstname, lastname</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>title, description, content</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Full text search index</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Full text search index</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3802,6 +3838,51 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3812,26 +3893,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3839,12 +3920,6 @@
     <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3881,20 +3956,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3949,51 +4030,6 @@
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="462">
@@ -5704,29 +5740,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="147"/>
-      <c r="P13" s="147"/>
-      <c r="Q13" s="147"/>
-      <c r="R13" s="147"/>
-      <c r="S13" s="147"/>
-      <c r="T13" s="147"/>
-      <c r="U13" s="147"/>
-      <c r="V13" s="147"/>
-      <c r="W13" s="147"/>
-      <c r="X13" s="147"/>
-      <c r="Y13" s="147"/>
-      <c r="Z13" s="147"/>
-      <c r="AA13" s="147"/>
-      <c r="AB13" s="147"/>
-      <c r="AC13" s="147"/>
-      <c r="AD13" s="147"/>
-      <c r="AE13" s="147"/>
-      <c r="AF13" s="147"/>
-      <c r="AG13" s="147"/>
-      <c r="AH13" s="147"/>
-      <c r="AI13" s="147"/>
-      <c r="AJ13" s="147"/>
-      <c r="AK13" s="147"/>
+      <c r="O13" s="162"/>
+      <c r="P13" s="162"/>
+      <c r="Q13" s="162"/>
+      <c r="R13" s="162"/>
+      <c r="S13" s="162"/>
+      <c r="T13" s="162"/>
+      <c r="U13" s="162"/>
+      <c r="V13" s="162"/>
+      <c r="W13" s="162"/>
+      <c r="X13" s="162"/>
+      <c r="Y13" s="162"/>
+      <c r="Z13" s="162"/>
+      <c r="AA13" s="162"/>
+      <c r="AB13" s="162"/>
+      <c r="AC13" s="162"/>
+      <c r="AD13" s="162"/>
+      <c r="AE13" s="162"/>
+      <c r="AF13" s="162"/>
+      <c r="AG13" s="162"/>
+      <c r="AH13" s="162"/>
+      <c r="AI13" s="162"/>
+      <c r="AJ13" s="162"/>
+      <c r="AK13" s="162"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -5758,29 +5794,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="147"/>
-      <c r="P14" s="147"/>
-      <c r="Q14" s="147"/>
-      <c r="R14" s="147"/>
-      <c r="S14" s="147"/>
-      <c r="T14" s="147"/>
-      <c r="U14" s="147"/>
-      <c r="V14" s="147"/>
-      <c r="W14" s="147"/>
-      <c r="X14" s="147"/>
-      <c r="Y14" s="147"/>
-      <c r="Z14" s="147"/>
-      <c r="AA14" s="147"/>
-      <c r="AB14" s="147"/>
-      <c r="AC14" s="147"/>
-      <c r="AD14" s="147"/>
-      <c r="AE14" s="147"/>
-      <c r="AF14" s="147"/>
-      <c r="AG14" s="147"/>
-      <c r="AH14" s="147"/>
-      <c r="AI14" s="147"/>
-      <c r="AJ14" s="147"/>
-      <c r="AK14" s="147"/>
+      <c r="O14" s="162"/>
+      <c r="P14" s="162"/>
+      <c r="Q14" s="162"/>
+      <c r="R14" s="162"/>
+      <c r="S14" s="162"/>
+      <c r="T14" s="162"/>
+      <c r="U14" s="162"/>
+      <c r="V14" s="162"/>
+      <c r="W14" s="162"/>
+      <c r="X14" s="162"/>
+      <c r="Y14" s="162"/>
+      <c r="Z14" s="162"/>
+      <c r="AA14" s="162"/>
+      <c r="AB14" s="162"/>
+      <c r="AC14" s="162"/>
+      <c r="AD14" s="162"/>
+      <c r="AE14" s="162"/>
+      <c r="AF14" s="162"/>
+      <c r="AG14" s="162"/>
+      <c r="AH14" s="162"/>
+      <c r="AI14" s="162"/>
+      <c r="AJ14" s="162"/>
+      <c r="AK14" s="162"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -5808,43 +5844,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="148" t="s">
+      <c r="K15" s="163" t="s">
         <v>112</v>
       </c>
-      <c r="L15" s="148"/>
-      <c r="M15" s="148"/>
-      <c r="N15" s="148"/>
-      <c r="O15" s="148"/>
-      <c r="P15" s="148"/>
-      <c r="Q15" s="148"/>
-      <c r="R15" s="148"/>
-      <c r="S15" s="148"/>
-      <c r="T15" s="148"/>
-      <c r="U15" s="148"/>
-      <c r="V15" s="148"/>
-      <c r="W15" s="148"/>
-      <c r="X15" s="148"/>
-      <c r="Y15" s="148"/>
-      <c r="Z15" s="148"/>
-      <c r="AA15" s="148"/>
-      <c r="AB15" s="148"/>
-      <c r="AC15" s="148"/>
-      <c r="AD15" s="148"/>
-      <c r="AE15" s="148"/>
-      <c r="AF15" s="148"/>
-      <c r="AG15" s="148"/>
-      <c r="AH15" s="148"/>
-      <c r="AI15" s="148"/>
-      <c r="AJ15" s="148"/>
-      <c r="AK15" s="148"/>
-      <c r="AL15" s="148"/>
-      <c r="AM15" s="148"/>
-      <c r="AN15" s="148"/>
-      <c r="AO15" s="148"/>
-      <c r="AP15" s="148"/>
-      <c r="AQ15" s="148"/>
-      <c r="AR15" s="148"/>
-      <c r="AS15" s="148"/>
+      <c r="L15" s="163"/>
+      <c r="M15" s="163"/>
+      <c r="N15" s="163"/>
+      <c r="O15" s="163"/>
+      <c r="P15" s="163"/>
+      <c r="Q15" s="163"/>
+      <c r="R15" s="163"/>
+      <c r="S15" s="163"/>
+      <c r="T15" s="163"/>
+      <c r="U15" s="163"/>
+      <c r="V15" s="163"/>
+      <c r="W15" s="163"/>
+      <c r="X15" s="163"/>
+      <c r="Y15" s="163"/>
+      <c r="Z15" s="163"/>
+      <c r="AA15" s="163"/>
+      <c r="AB15" s="163"/>
+      <c r="AC15" s="163"/>
+      <c r="AD15" s="163"/>
+      <c r="AE15" s="163"/>
+      <c r="AF15" s="163"/>
+      <c r="AG15" s="163"/>
+      <c r="AH15" s="163"/>
+      <c r="AI15" s="163"/>
+      <c r="AJ15" s="163"/>
+      <c r="AK15" s="163"/>
+      <c r="AL15" s="163"/>
+      <c r="AM15" s="163"/>
+      <c r="AN15" s="163"/>
+      <c r="AO15" s="163"/>
+      <c r="AP15" s="163"/>
+      <c r="AQ15" s="163"/>
+      <c r="AR15" s="163"/>
+      <c r="AS15" s="163"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -5864,41 +5900,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="148"/>
-      <c r="L16" s="148"/>
-      <c r="M16" s="148"/>
-      <c r="N16" s="148"/>
-      <c r="O16" s="148"/>
-      <c r="P16" s="148"/>
-      <c r="Q16" s="148"/>
-      <c r="R16" s="148"/>
-      <c r="S16" s="148"/>
-      <c r="T16" s="148"/>
-      <c r="U16" s="148"/>
-      <c r="V16" s="148"/>
-      <c r="W16" s="148"/>
-      <c r="X16" s="148"/>
-      <c r="Y16" s="148"/>
-      <c r="Z16" s="148"/>
-      <c r="AA16" s="148"/>
-      <c r="AB16" s="148"/>
-      <c r="AC16" s="148"/>
-      <c r="AD16" s="148"/>
-      <c r="AE16" s="148"/>
-      <c r="AF16" s="148"/>
-      <c r="AG16" s="148"/>
-      <c r="AH16" s="148"/>
-      <c r="AI16" s="148"/>
-      <c r="AJ16" s="148"/>
-      <c r="AK16" s="148"/>
-      <c r="AL16" s="148"/>
-      <c r="AM16" s="148"/>
-      <c r="AN16" s="148"/>
-      <c r="AO16" s="148"/>
-      <c r="AP16" s="148"/>
-      <c r="AQ16" s="148"/>
-      <c r="AR16" s="148"/>
-      <c r="AS16" s="148"/>
+      <c r="K16" s="163"/>
+      <c r="L16" s="163"/>
+      <c r="M16" s="163"/>
+      <c r="N16" s="163"/>
+      <c r="O16" s="163"/>
+      <c r="P16" s="163"/>
+      <c r="Q16" s="163"/>
+      <c r="R16" s="163"/>
+      <c r="S16" s="163"/>
+      <c r="T16" s="163"/>
+      <c r="U16" s="163"/>
+      <c r="V16" s="163"/>
+      <c r="W16" s="163"/>
+      <c r="X16" s="163"/>
+      <c r="Y16" s="163"/>
+      <c r="Z16" s="163"/>
+      <c r="AA16" s="163"/>
+      <c r="AB16" s="163"/>
+      <c r="AC16" s="163"/>
+      <c r="AD16" s="163"/>
+      <c r="AE16" s="163"/>
+      <c r="AF16" s="163"/>
+      <c r="AG16" s="163"/>
+      <c r="AH16" s="163"/>
+      <c r="AI16" s="163"/>
+      <c r="AJ16" s="163"/>
+      <c r="AK16" s="163"/>
+      <c r="AL16" s="163"/>
+      <c r="AM16" s="163"/>
+      <c r="AN16" s="163"/>
+      <c r="AO16" s="163"/>
+      <c r="AP16" s="163"/>
+      <c r="AQ16" s="163"/>
+      <c r="AR16" s="163"/>
+      <c r="AS16" s="163"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6487,14 +6523,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="149" t="s">
+      <c r="AN27" s="164" t="s">
         <v>113</v>
       </c>
-      <c r="AO27" s="149"/>
-      <c r="AP27" s="149"/>
-      <c r="AQ27" s="149"/>
-      <c r="AR27" s="149"/>
-      <c r="AS27" s="149"/>
+      <c r="AO27" s="164"/>
+      <c r="AP27" s="164"/>
+      <c r="AQ27" s="164"/>
+      <c r="AR27" s="164"/>
+      <c r="AS27" s="164"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -7241,7 +7277,7 @@
   </sheetPr>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -7253,11 +7289,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12" thickBot="1">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="165" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
     </row>
     <row r="2" spans="1:3" ht="12" thickBot="1">
       <c r="A2" s="118" t="s">
@@ -7520,8 +7556,8 @@
   </sheetPr>
   <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -7554,101 +7590,101 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="151" t="s">
+      <c r="C2" s="187" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="152"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="151"/>
-      <c r="G2" s="155"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="188"/>
     </row>
     <row r="3" spans="1:22" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="153"/>
-      <c r="D3" s="154"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="156" t="s">
+      <c r="F3" s="189" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="157"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:22" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="191" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="154"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="153"/>
-      <c r="G4" s="157"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:22" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="191" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="154"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="157"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:22" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="191" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="154"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="157"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:22" ht="13">
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:22">
-      <c r="B8" s="165"/>
-      <c r="C8" s="166"/>
-      <c r="D8" s="166"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="166"/>
-      <c r="G8" s="167"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:22">
-      <c r="B9" s="168"/>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="167"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:22" ht="12" thickBot="1">
-      <c r="B10" s="169"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="170"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="171"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="12" spans="1:22" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8009,39 +8045,39 @@
       <c r="A25" s="59">
         <v>12</v>
       </c>
-      <c r="B25" s="202" t="s">
+      <c r="B25" s="152" t="s">
         <v>183</v>
       </c>
-      <c r="C25" s="203" t="s">
+      <c r="C25" s="153" t="s">
         <v>184</v>
       </c>
-      <c r="D25" s="203" t="s">
+      <c r="D25" s="153" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="204" t="s">
+      <c r="E25" s="154" t="s">
         <v>0</v>
       </c>
-      <c r="F25" s="205"/>
-      <c r="G25" s="206"/>
+      <c r="F25" s="155"/>
+      <c r="G25" s="156"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="69">
         <v>13</v>
       </c>
-      <c r="B26" s="197" t="s">
+      <c r="B26" s="147" t="s">
         <v>205</v>
       </c>
-      <c r="C26" s="198" t="s">
+      <c r="C26" s="148" t="s">
         <v>206</v>
       </c>
-      <c r="D26" s="198" t="s">
+      <c r="D26" s="148" t="s">
         <v>147</v>
       </c>
-      <c r="E26" s="199" t="s">
+      <c r="E26" s="149" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="200"/>
-      <c r="G26" s="201" t="s">
+      <c r="F26" s="150"/>
+      <c r="G26" s="151" t="s">
         <v>173</v>
       </c>
     </row>
@@ -8049,7 +8085,7 @@
       <c r="A27" s="70">
         <v>14</v>
       </c>
-      <c r="B27" s="207" t="s">
+      <c r="B27" s="157" t="s">
         <v>207</v>
       </c>
       <c r="C27" s="68" t="s">
@@ -8058,11 +8094,11 @@
       <c r="D27" s="68" t="s">
         <v>147</v>
       </c>
-      <c r="E27" s="208" t="s">
+      <c r="E27" s="158" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="209"/>
-      <c r="G27" s="210" t="s">
+      <c r="F27" s="159"/>
+      <c r="G27" s="160" t="s">
         <v>173</v>
       </c>
     </row>
@@ -8078,10 +8114,10 @@
       <c r="B30" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="158" t="s">
+      <c r="C30" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="159"/>
+      <c r="D30" s="174"/>
       <c r="E30" s="34" t="s">
         <v>33</v>
       </c>
@@ -8099,10 +8135,10 @@
       <c r="B31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="172" t="s">
+      <c r="C31" s="185" t="s">
         <v>109</v>
       </c>
-      <c r="D31" s="173"/>
+      <c r="D31" s="186"/>
       <c r="E31" s="46" t="s">
         <v>3</v>
       </c>
@@ -8115,20 +8151,30 @@
       <c r="A32" s="57">
         <v>2</v>
       </c>
-      <c r="B32" s="51"/>
-      <c r="C32" s="177"/>
-      <c r="D32" s="178"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="53"/>
+      <c r="B32" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="C32" s="171" t="s">
+        <v>238</v>
+      </c>
+      <c r="D32" s="172"/>
+      <c r="E32" s="52" t="s">
+        <v>239</v>
+      </c>
+      <c r="F32" s="52" t="s">
+        <v>239</v>
+      </c>
+      <c r="G32" s="53" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="13" customHeight="1" thickBot="1">
       <c r="A33" s="56">
         <v>3</v>
       </c>
       <c r="B33" s="54"/>
-      <c r="C33" s="175"/>
-      <c r="D33" s="176"/>
+      <c r="C33" s="169"/>
+      <c r="D33" s="170"/>
       <c r="E33" s="58"/>
       <c r="F33" s="58"/>
       <c r="G33" s="55"/>
@@ -8145,14 +8191,14 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="160" t="s">
+      <c r="C36" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="161"/>
-      <c r="E36" s="160" t="s">
+      <c r="D36" s="167"/>
+      <c r="E36" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F36" s="174"/>
+      <c r="F36" s="168"/>
       <c r="G36" s="38" t="s">
         <v>38</v>
       </c>
@@ -8169,40 +8215,40 @@
       <c r="B39" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="160" t="s">
+      <c r="C39" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="161"/>
-      <c r="E39" s="160" t="s">
+      <c r="D39" s="167"/>
+      <c r="E39" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="174"/>
+      <c r="F39" s="168"/>
       <c r="G39" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C31:D31"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -8254,103 +8300,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="151" t="s">
+      <c r="C2" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="152"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="151" t="s">
+      <c r="F2" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="155"/>
+      <c r="G2" s="188"/>
     </row>
     <row r="3" spans="1:11" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="153"/>
-      <c r="D3" s="154"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="153" t="s">
+      <c r="F3" s="191" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="157"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:11" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="191" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="154"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="153"/>
-      <c r="G4" s="157"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:11" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="191" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="154"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="157"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:11" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="191" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="154"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="157"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:11" ht="13">
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="165"/>
-      <c r="C8" s="166"/>
-      <c r="D8" s="166"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="166"/>
-      <c r="G8" s="167"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="168"/>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="167"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:11" ht="12" thickBot="1">
-      <c r="B10" s="169"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="170"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="171"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="12" spans="1:11" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8572,10 +8618,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="158" t="s">
+      <c r="C24" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="159"/>
+      <c r="D24" s="174"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -8593,10 +8639,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="172" t="s">
+      <c r="C25" s="185" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="173"/>
+      <c r="D25" s="186"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -8610,10 +8656,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="181" t="s">
+      <c r="C26" s="196" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="182"/>
+      <c r="D26" s="197"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -8632,14 +8678,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="160" t="s">
+      <c r="C29" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="161"/>
-      <c r="E29" s="160" t="s">
+      <c r="D29" s="167"/>
+      <c r="E29" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="174"/>
+      <c r="F29" s="168"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -8656,14 +8702,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="160" t="s">
+      <c r="C32" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="161"/>
-      <c r="E32" s="160" t="s">
+      <c r="D32" s="167"/>
+      <c r="E32" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="174"/>
+      <c r="F32" s="168"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -8673,29 +8719,20 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="179" t="s">
+      <c r="C33" s="194" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="180"/>
-      <c r="E33" s="181" t="s">
+      <c r="D33" s="195"/>
+      <c r="E33" s="196" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="182"/>
+      <c r="F33" s="197"/>
       <c r="G33" s="28" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -8708,6 +8745,15 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8755,105 +8801,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="151" t="s">
+      <c r="C2" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="152"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="151" t="s">
+      <c r="F2" s="187" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="155"/>
+      <c r="G2" s="188"/>
     </row>
     <row r="3" spans="1:7" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="153"/>
-      <c r="D3" s="154"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="153" t="s">
+      <c r="F3" s="191" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="157"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:7" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="191" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="154"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="153"/>
-      <c r="G4" s="157"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:7" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="191" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="154"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="157"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:7" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="191" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="154"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="157"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:7" ht="13">
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="165" t="s">
+      <c r="B8" s="178" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="166"/>
-      <c r="D8" s="166"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="166"/>
-      <c r="G8" s="167"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="168"/>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="167"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:7" ht="12" thickBot="1">
-      <c r="B10" s="169"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="170"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="171"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="12" spans="1:7" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8958,10 +9004,10 @@
       <c r="B19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="158" t="s">
+      <c r="C19" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="159"/>
+      <c r="D19" s="174"/>
       <c r="E19" s="34" t="s">
         <v>33</v>
       </c>
@@ -8979,10 +9025,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="172" t="s">
+      <c r="C20" s="185" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="173"/>
+      <c r="D20" s="186"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -8996,10 +9042,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="179" t="s">
+      <c r="C21" s="194" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="180"/>
+      <c r="D21" s="195"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
         <v>3</v>
@@ -9018,14 +9064,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="160" t="s">
+      <c r="C24" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="161"/>
-      <c r="E24" s="160" t="s">
+      <c r="D24" s="167"/>
+      <c r="E24" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="174"/>
+      <c r="F24" s="168"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -9042,14 +9088,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="160" t="s">
+      <c r="C27" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="161"/>
-      <c r="E27" s="160" t="s">
+      <c r="D27" s="167"/>
+      <c r="E27" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="174"/>
+      <c r="F27" s="168"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -9059,23 +9105,14 @@
         <v>1</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="179"/>
-      <c r="D28" s="180"/>
-      <c r="E28" s="181"/>
-      <c r="F28" s="182"/>
+      <c r="C28" s="194"/>
+      <c r="D28" s="195"/>
+      <c r="E28" s="196"/>
+      <c r="F28" s="197"/>
       <c r="G28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -9088,6 +9125,15 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9135,103 +9181,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="151" t="s">
+      <c r="C2" s="187" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="152"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="185" t="s">
+      <c r="F2" s="200" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="186"/>
+      <c r="G2" s="201"/>
     </row>
     <row r="3" spans="1:14" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="153"/>
-      <c r="D3" s="154"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="156" t="s">
+      <c r="F3" s="189" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="157"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:14" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="191" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="154"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="153"/>
-      <c r="G4" s="157"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:14" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="191" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="154"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="157"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:14" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="191" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="154"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="157"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:14" ht="13">
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="165"/>
-      <c r="C8" s="166"/>
-      <c r="D8" s="166"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="166"/>
-      <c r="G8" s="167"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="168"/>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="167"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:14" ht="12" thickBot="1">
-      <c r="B10" s="169"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="170"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="171"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -9447,10 +9493,10 @@
       <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="158" t="s">
+      <c r="C21" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="159"/>
+      <c r="D21" s="174"/>
       <c r="E21" s="34" t="s">
         <v>33</v>
       </c>
@@ -9474,10 +9520,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="172" t="s">
+      <c r="C22" s="185" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="173"/>
+      <c r="D22" s="186"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -9497,10 +9543,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="177" t="s">
+      <c r="C23" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="178"/>
+      <c r="D23" s="172"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -9518,10 +9564,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="179" t="s">
+      <c r="C24" s="194" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="180"/>
+      <c r="D24" s="195"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -9560,14 +9606,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="160" t="s">
+      <c r="C27" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="161"/>
-      <c r="E27" s="160" t="s">
+      <c r="D27" s="167"/>
+      <c r="E27" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="174"/>
+      <c r="F27" s="168"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -9604,14 +9650,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="160" t="s">
+      <c r="C30" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="161"/>
-      <c r="E30" s="160" t="s">
+      <c r="D30" s="167"/>
+      <c r="E30" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="174"/>
+      <c r="F30" s="168"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -9627,14 +9673,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="172" t="s">
+      <c r="C31" s="185" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="173"/>
-      <c r="E31" s="177" t="s">
+      <c r="D31" s="186"/>
+      <c r="E31" s="171" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="178"/>
+      <c r="F31" s="172"/>
       <c r="G31" s="53" t="s">
         <v>76</v>
       </c>
@@ -9650,14 +9696,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="183" t="s">
+      <c r="C32" s="198" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="184"/>
-      <c r="E32" s="181" t="s">
+      <c r="D32" s="199"/>
+      <c r="E32" s="196" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="182"/>
+      <c r="F32" s="197"/>
       <c r="G32" s="55" t="s">
         <v>52</v>
       </c>
@@ -9710,6 +9756,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="C31:D31"/>
@@ -9726,14 +9780,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9757,8 +9803,8 @@
   </sheetPr>
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="K3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -9788,101 +9834,101 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="151" t="s">
+      <c r="C2" s="187" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="152"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="151"/>
-      <c r="G2" s="155"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="188"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="153"/>
-      <c r="D3" s="154"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="156" t="s">
+      <c r="F3" s="189" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="157"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="191" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="154"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="153"/>
-      <c r="G4" s="157"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="191" t="s">
         <v>212</v>
       </c>
-      <c r="D5" s="154"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="157"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="191" t="s">
         <v>213</v>
       </c>
-      <c r="D6" s="154"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="157"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:19" ht="13">
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="165"/>
-      <c r="C8" s="166"/>
-      <c r="D8" s="166"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="166"/>
-      <c r="G8" s="167"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="168"/>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="167"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:19" ht="12" thickBot="1">
-      <c r="B10" s="169"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="170"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="171"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="12" spans="1:19" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10215,10 +10261,10 @@
       <c r="B26" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="158" t="s">
+      <c r="C26" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="159"/>
+      <c r="D26" s="174"/>
       <c r="E26" s="34" t="s">
         <v>33</v>
       </c>
@@ -10236,10 +10282,10 @@
       <c r="B27" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="172" t="s">
+      <c r="C27" s="185" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="173"/>
+      <c r="D27" s="186"/>
       <c r="E27" s="46" t="s">
         <v>3</v>
       </c>
@@ -10252,20 +10298,30 @@
       <c r="A28" s="57">
         <v>2</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="177"/>
-      <c r="D28" s="178"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="53"/>
+      <c r="B28" s="51" t="s">
+        <v>240</v>
+      </c>
+      <c r="C28" s="171" t="s">
+        <v>241</v>
+      </c>
+      <c r="D28" s="172"/>
+      <c r="E28" s="52" t="s">
+        <v>242</v>
+      </c>
+      <c r="F28" s="52" t="s">
+        <v>243</v>
+      </c>
+      <c r="G28" s="53" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="13" customHeight="1" thickBot="1">
       <c r="A29" s="56">
         <v>3</v>
       </c>
       <c r="B29" s="54"/>
-      <c r="C29" s="175"/>
-      <c r="D29" s="176"/>
+      <c r="C29" s="169"/>
+      <c r="D29" s="170"/>
       <c r="E29" s="58"/>
       <c r="F29" s="58"/>
       <c r="G29" s="55"/>
@@ -10282,14 +10338,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="160" t="s">
+      <c r="C32" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="161"/>
-      <c r="E32" s="160" t="s">
+      <c r="D32" s="167"/>
+      <c r="E32" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="174"/>
+      <c r="F32" s="168"/>
       <c r="G32" s="38" t="s">
         <v>38</v>
       </c>
@@ -10299,14 +10355,14 @@
         <v>1</v>
       </c>
       <c r="B33" s="19"/>
-      <c r="C33" s="172" t="s">
+      <c r="C33" s="185" t="s">
         <v>137</v>
       </c>
-      <c r="D33" s="173"/>
-      <c r="E33" s="187" t="s">
+      <c r="D33" s="186"/>
+      <c r="E33" s="202" t="s">
         <v>151</v>
       </c>
-      <c r="F33" s="188"/>
+      <c r="F33" s="203"/>
       <c r="G33" s="20" t="s">
         <v>152</v>
       </c>
@@ -10323,20 +10379,30 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="160" t="s">
+      <c r="C36" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="161"/>
-      <c r="E36" s="160" t="s">
+      <c r="D36" s="167"/>
+      <c r="E36" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="174"/>
+      <c r="F36" s="168"/>
       <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -10349,16 +10415,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10412,101 +10468,101 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="151" t="s">
+      <c r="C2" s="187" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="152"/>
+      <c r="D2" s="192"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="151"/>
-      <c r="G2" s="155"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="188"/>
     </row>
     <row r="3" spans="1:18" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="153"/>
-      <c r="D3" s="154"/>
+      <c r="C3" s="191"/>
+      <c r="D3" s="193"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="156" t="s">
+      <c r="F3" s="189" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="157"/>
+      <c r="G3" s="190"/>
     </row>
     <row r="4" spans="1:18" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="191" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="154"/>
+      <c r="D4" s="193"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="153"/>
-      <c r="G4" s="157"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="190"/>
     </row>
     <row r="5" spans="1:18" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="191" t="s">
         <v>222</v>
       </c>
-      <c r="D5" s="154"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="153"/>
-      <c r="G5" s="157"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="190"/>
     </row>
     <row r="6" spans="1:18" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="191" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="154"/>
+      <c r="D6" s="193"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="157"/>
+      <c r="F6" s="191"/>
+      <c r="G6" s="190"/>
     </row>
     <row r="7" spans="1:18" ht="13">
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="175" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="B8" s="165"/>
-      <c r="C8" s="166"/>
-      <c r="D8" s="166"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="166"/>
-      <c r="G8" s="167"/>
+      <c r="B8" s="178"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="168"/>
-      <c r="C9" s="166"/>
-      <c r="D9" s="166"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="167"/>
+      <c r="B9" s="181"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
     </row>
     <row r="10" spans="1:18" ht="12" thickBot="1">
-      <c r="B10" s="169"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="170"/>
-      <c r="E10" s="170"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="171"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="183"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="184"/>
     </row>
     <row r="12" spans="1:18" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10588,10 +10644,10 @@
       <c r="J14" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="K14" s="211">
+      <c r="K14" s="161">
         <v>1</v>
       </c>
-      <c r="L14" s="211">
+      <c r="L14" s="161">
         <v>1</v>
       </c>
       <c r="M14" s="127" t="s">
@@ -10630,10 +10686,10 @@
       <c r="J15" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="K15" s="211">
+      <c r="K15" s="161">
         <v>1</v>
       </c>
-      <c r="L15" s="211">
+      <c r="L15" s="161">
         <v>2</v>
       </c>
       <c r="M15" s="127" t="s">
@@ -10765,10 +10821,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="158" t="s">
+      <c r="C24" s="173" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="159"/>
+      <c r="D24" s="174"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -10786,10 +10842,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="172" t="s">
+      <c r="C25" s="185" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="173"/>
+      <c r="D25" s="186"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -10803,8 +10859,8 @@
         <v>2</v>
       </c>
       <c r="B26" s="51"/>
-      <c r="C26" s="177"/>
-      <c r="D26" s="178"/>
+      <c r="C26" s="171"/>
+      <c r="D26" s="172"/>
       <c r="E26" s="46"/>
       <c r="F26" s="46"/>
       <c r="G26" s="20"/>
@@ -10814,8 +10870,8 @@
         <v>3</v>
       </c>
       <c r="B27" s="54"/>
-      <c r="C27" s="175"/>
-      <c r="D27" s="176"/>
+      <c r="C27" s="169"/>
+      <c r="D27" s="170"/>
       <c r="E27" s="58"/>
       <c r="F27" s="58"/>
       <c r="G27" s="55"/>
@@ -10832,14 +10888,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="160" t="s">
+      <c r="C30" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="161"/>
-      <c r="E30" s="160" t="s">
+      <c r="D30" s="167"/>
+      <c r="E30" s="166" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="174"/>
+      <c r="F30" s="168"/>
       <c r="G30" s="38" t="s">
         <v>38</v>
       </c>
@@ -10849,14 +10905,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="19"/>
-      <c r="C31" s="187" t="s">
+      <c r="C31" s="202" t="s">
         <v>216</v>
       </c>
-      <c r="D31" s="188"/>
-      <c r="E31" s="191" t="s">
+      <c r="D31" s="203"/>
+      <c r="E31" s="206" t="s">
         <v>199</v>
       </c>
-      <c r="F31" s="192"/>
+      <c r="F31" s="207"/>
       <c r="G31" s="20" t="s">
         <v>152</v>
       </c>
@@ -10866,14 +10922,14 @@
         <v>1</v>
       </c>
       <c r="B32" s="19"/>
-      <c r="C32" s="189" t="s">
+      <c r="C32" s="204" t="s">
         <v>218</v>
       </c>
-      <c r="D32" s="190"/>
-      <c r="E32" s="193" t="s">
+      <c r="D32" s="205"/>
+      <c r="E32" s="208" t="s">
         <v>213</v>
       </c>
-      <c r="F32" s="194"/>
+      <c r="F32" s="209"/>
       <c r="G32" s="20" t="s">
         <v>217</v>
       </c>
@@ -10883,10 +10939,10 @@
         <v>3</v>
       </c>
       <c r="B33" s="54"/>
-      <c r="C33" s="175"/>
-      <c r="D33" s="176"/>
-      <c r="E33" s="195"/>
-      <c r="F33" s="196"/>
+      <c r="C33" s="169"/>
+      <c r="D33" s="170"/>
+      <c r="E33" s="210"/>
+      <c r="F33" s="211"/>
       <c r="G33" s="55"/>
     </row>
     <row r="35" spans="1:7" ht="12" thickBot="1">
@@ -10901,26 +10957,28 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="160" t="s">
+      <c r="C36" s="166" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="161"/>
-      <c r="E36" s="160" t="s">
+      <c r="D36" s="167"/>
+      <c r="E36" s="166" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="161"/>
+      <c r="F36" s="167"/>
       <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="F5:G5"/>
@@ -10933,14 +10991,12 @@
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed space & change index name to FULLTEXT
</commit_message>
<xml_diff>
--- a/doc/detail_design/db/MiniBlog_Database_Design.xlsx
+++ b/doc/detail_design/db/MiniBlog_Database_Design.xlsx
@@ -907,22 +907,10 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>username</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>username, firstname, lastname</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>no</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>title</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>title, description, content</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -940,6 +928,18 @@
   </si>
   <si>
     <t>Full text search index</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>FULLTEXT</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>FULLTEXT</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>No</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -3893,12 +3893,75 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3913,69 +3976,6 @@
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -7557,7 +7557,7 @@
   <dimension ref="A1:V39"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -7590,101 +7590,101 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="166" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="192"/>
+      <c r="D2" s="167"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="187"/>
-      <c r="G2" s="188"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="170"/>
     </row>
     <row r="3" spans="1:22" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="191"/>
-      <c r="D3" s="193"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="169"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="189" t="s">
+      <c r="F3" s="171" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="190"/>
+      <c r="G3" s="172"/>
     </row>
     <row r="4" spans="1:22" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="191" t="s">
+      <c r="C4" s="168" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="193"/>
+      <c r="D4" s="169"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="191"/>
-      <c r="G4" s="190"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="172"/>
     </row>
     <row r="5" spans="1:22" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="191" t="s">
+      <c r="C5" s="168" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="193"/>
+      <c r="D5" s="169"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="190"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="172"/>
     </row>
     <row r="6" spans="1:22" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="191" t="s">
+      <c r="C6" s="168" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="193"/>
+      <c r="D6" s="169"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="191"/>
-      <c r="G6" s="190"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="172"/>
     </row>
     <row r="7" spans="1:22" ht="13">
-      <c r="B7" s="175" t="s">
+      <c r="B7" s="177" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="177"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="178"/>
+      <c r="E7" s="178"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="179"/>
     </row>
     <row r="8" spans="1:22">
-      <c r="B8" s="178"/>
-      <c r="C8" s="179"/>
-      <c r="D8" s="179"/>
-      <c r="E8" s="179"/>
-      <c r="F8" s="179"/>
-      <c r="G8" s="180"/>
+      <c r="B8" s="180"/>
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="182"/>
     </row>
     <row r="9" spans="1:22">
-      <c r="B9" s="181"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
-      <c r="G9" s="180"/>
+      <c r="B9" s="183"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="182"/>
     </row>
     <row r="10" spans="1:22" ht="12" thickBot="1">
-      <c r="B10" s="182"/>
-      <c r="C10" s="183"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="184"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
+      <c r="F10" s="185"/>
+      <c r="G10" s="186"/>
     </row>
     <row r="12" spans="1:22" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8135,10 +8135,10 @@
       <c r="B31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="185" t="s">
+      <c r="C31" s="187" t="s">
         <v>109</v>
       </c>
-      <c r="D31" s="186"/>
+      <c r="D31" s="188"/>
       <c r="E31" s="46" t="s">
         <v>3</v>
       </c>
@@ -8152,20 +8152,20 @@
         <v>2</v>
       </c>
       <c r="B32" s="51" t="s">
+        <v>244</v>
+      </c>
+      <c r="C32" s="192" t="s">
         <v>237</v>
       </c>
-      <c r="C32" s="171" t="s">
-        <v>238</v>
-      </c>
-      <c r="D32" s="172"/>
+      <c r="D32" s="193"/>
       <c r="E32" s="52" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="F32" s="52" t="s">
-        <v>239</v>
+        <v>245</v>
       </c>
       <c r="G32" s="53" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="13" customHeight="1" thickBot="1">
@@ -8173,8 +8173,8 @@
         <v>3</v>
       </c>
       <c r="B33" s="54"/>
-      <c r="C33" s="169"/>
-      <c r="D33" s="170"/>
+      <c r="C33" s="190"/>
+      <c r="D33" s="191"/>
       <c r="E33" s="58"/>
       <c r="F33" s="58"/>
       <c r="G33" s="55"/>
@@ -8191,14 +8191,14 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="166" t="s">
+      <c r="C36" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="167"/>
-      <c r="E36" s="166" t="s">
+      <c r="D36" s="176"/>
+      <c r="E36" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="F36" s="168"/>
+      <c r="F36" s="189"/>
       <c r="G36" s="38" t="s">
         <v>38</v>
       </c>
@@ -8215,40 +8215,40 @@
       <c r="B39" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="166" t="s">
+      <c r="C39" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="167"/>
-      <c r="E39" s="166" t="s">
+      <c r="D39" s="176"/>
+      <c r="E39" s="175" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="168"/>
+      <c r="F39" s="189"/>
       <c r="G39" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -8300,103 +8300,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="166" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="192"/>
+      <c r="D2" s="167"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="187" t="s">
+      <c r="F2" s="166" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="188"/>
+      <c r="G2" s="170"/>
     </row>
     <row r="3" spans="1:11" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="191"/>
-      <c r="D3" s="193"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="169"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="191" t="s">
+      <c r="F3" s="168" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="190"/>
+      <c r="G3" s="172"/>
     </row>
     <row r="4" spans="1:11" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="191" t="s">
+      <c r="C4" s="168" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="193"/>
+      <c r="D4" s="169"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="191"/>
-      <c r="G4" s="190"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="172"/>
     </row>
     <row r="5" spans="1:11" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="191" t="s">
+      <c r="C5" s="168" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="193"/>
+      <c r="D5" s="169"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="190"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="172"/>
     </row>
     <row r="6" spans="1:11" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="191" t="s">
+      <c r="C6" s="168" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="193"/>
+      <c r="D6" s="169"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="191"/>
-      <c r="G6" s="190"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="172"/>
     </row>
     <row r="7" spans="1:11" ht="13">
-      <c r="B7" s="175" t="s">
+      <c r="B7" s="177" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="177"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="178"/>
+      <c r="E7" s="178"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="179"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="178"/>
-      <c r="C8" s="179"/>
-      <c r="D8" s="179"/>
-      <c r="E8" s="179"/>
-      <c r="F8" s="179"/>
-      <c r="G8" s="180"/>
+      <c r="B8" s="180"/>
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="182"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="181"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
-      <c r="G9" s="180"/>
+      <c r="B9" s="183"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="182"/>
     </row>
     <row r="10" spans="1:11" ht="12" thickBot="1">
-      <c r="B10" s="182"/>
-      <c r="C10" s="183"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="184"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
+      <c r="F10" s="185"/>
+      <c r="G10" s="186"/>
     </row>
     <row r="12" spans="1:11" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8639,10 +8639,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="185" t="s">
+      <c r="C25" s="187" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="186"/>
+      <c r="D25" s="188"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -8678,14 +8678,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="166" t="s">
+      <c r="C29" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="167"/>
-      <c r="E29" s="166" t="s">
+      <c r="D29" s="176"/>
+      <c r="E29" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="168"/>
+      <c r="F29" s="189"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -8702,14 +8702,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="166" t="s">
+      <c r="C32" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="167"/>
-      <c r="E32" s="166" t="s">
+      <c r="D32" s="176"/>
+      <c r="E32" s="175" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="168"/>
+      <c r="F32" s="189"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -8733,6 +8733,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -8745,15 +8754,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8801,105 +8801,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="166" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="192"/>
+      <c r="D2" s="167"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="187" t="s">
+      <c r="F2" s="166" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="188"/>
+      <c r="G2" s="170"/>
     </row>
     <row r="3" spans="1:7" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="191"/>
-      <c r="D3" s="193"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="169"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="191" t="s">
+      <c r="F3" s="168" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="190"/>
+      <c r="G3" s="172"/>
     </row>
     <row r="4" spans="1:7" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="191" t="s">
+      <c r="C4" s="168" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="193"/>
+      <c r="D4" s="169"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="191"/>
-      <c r="G4" s="190"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="172"/>
     </row>
     <row r="5" spans="1:7" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="191" t="s">
+      <c r="C5" s="168" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="193"/>
+      <c r="D5" s="169"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="190"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="172"/>
     </row>
     <row r="6" spans="1:7" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="191" t="s">
+      <c r="C6" s="168" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="193"/>
+      <c r="D6" s="169"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="191"/>
-      <c r="G6" s="190"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="172"/>
     </row>
     <row r="7" spans="1:7" ht="13">
-      <c r="B7" s="175" t="s">
+      <c r="B7" s="177" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="177"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="178"/>
+      <c r="E7" s="178"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="179"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="178" t="s">
+      <c r="B8" s="180" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="179"/>
-      <c r="D8" s="179"/>
-      <c r="E8" s="179"/>
-      <c r="F8" s="179"/>
-      <c r="G8" s="180"/>
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="182"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="181"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
-      <c r="G9" s="180"/>
+      <c r="B9" s="183"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="182"/>
     </row>
     <row r="10" spans="1:7" ht="12" thickBot="1">
-      <c r="B10" s="182"/>
-      <c r="C10" s="183"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="184"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
+      <c r="F10" s="185"/>
+      <c r="G10" s="186"/>
     </row>
     <row r="12" spans="1:7" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9025,10 +9025,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="185" t="s">
+      <c r="C20" s="187" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="186"/>
+      <c r="D20" s="188"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -9064,14 +9064,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="166" t="s">
+      <c r="C24" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="167"/>
-      <c r="E24" s="166" t="s">
+      <c r="D24" s="176"/>
+      <c r="E24" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="168"/>
+      <c r="F24" s="189"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -9088,14 +9088,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="166" t="s">
+      <c r="C27" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="167"/>
-      <c r="E27" s="166" t="s">
+      <c r="D27" s="176"/>
+      <c r="E27" s="175" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="168"/>
+      <c r="F27" s="189"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -9113,6 +9113,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -9125,15 +9134,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9181,10 +9181,10 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="166" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="192"/>
+      <c r="D2" s="167"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
@@ -9197,87 +9197,87 @@
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="191"/>
-      <c r="D3" s="193"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="169"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="189" t="s">
+      <c r="F3" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="190"/>
+      <c r="G3" s="172"/>
     </row>
     <row r="4" spans="1:14" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="191" t="s">
+      <c r="C4" s="168" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="193"/>
+      <c r="D4" s="169"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="191"/>
-      <c r="G4" s="190"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="172"/>
     </row>
     <row r="5" spans="1:14" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="191" t="s">
+      <c r="C5" s="168" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="193"/>
+      <c r="D5" s="169"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="190"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="172"/>
     </row>
     <row r="6" spans="1:14" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="191" t="s">
+      <c r="C6" s="168" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="193"/>
+      <c r="D6" s="169"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="191"/>
-      <c r="G6" s="190"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="172"/>
     </row>
     <row r="7" spans="1:14" ht="13">
-      <c r="B7" s="175" t="s">
+      <c r="B7" s="177" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="177"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="178"/>
+      <c r="E7" s="178"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="179"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="178"/>
-      <c r="C8" s="179"/>
-      <c r="D8" s="179"/>
-      <c r="E8" s="179"/>
-      <c r="F8" s="179"/>
-      <c r="G8" s="180"/>
+      <c r="B8" s="180"/>
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="182"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="181"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
-      <c r="G9" s="180"/>
+      <c r="B9" s="183"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="182"/>
     </row>
     <row r="10" spans="1:14" ht="12" thickBot="1">
-      <c r="B10" s="182"/>
-      <c r="C10" s="183"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="184"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
+      <c r="F10" s="185"/>
+      <c r="G10" s="186"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -9520,10 +9520,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="185" t="s">
+      <c r="C22" s="187" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="186"/>
+      <c r="D22" s="188"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -9543,10 +9543,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="171" t="s">
+      <c r="C23" s="192" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="172"/>
+      <c r="D23" s="193"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -9606,14 +9606,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="166" t="s">
+      <c r="C27" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="167"/>
-      <c r="E27" s="166" t="s">
+      <c r="D27" s="176"/>
+      <c r="E27" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="168"/>
+      <c r="F27" s="189"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -9650,14 +9650,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="166" t="s">
+      <c r="C30" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="167"/>
-      <c r="E30" s="166" t="s">
+      <c r="D30" s="176"/>
+      <c r="E30" s="175" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="168"/>
+      <c r="F30" s="189"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -9673,14 +9673,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="185" t="s">
+      <c r="C31" s="187" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="186"/>
-      <c r="E31" s="171" t="s">
+      <c r="D31" s="188"/>
+      <c r="E31" s="192" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="172"/>
+      <c r="F31" s="193"/>
       <c r="G31" s="53" t="s">
         <v>76</v>
       </c>
@@ -9756,14 +9756,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="C31:D31"/>
@@ -9780,6 +9772,14 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9834,101 +9834,101 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="166" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="192"/>
+      <c r="D2" s="167"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="187"/>
-      <c r="G2" s="188"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="170"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="191"/>
-      <c r="D3" s="193"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="169"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="189" t="s">
+      <c r="F3" s="171" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="190"/>
+      <c r="G3" s="172"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="191" t="s">
+      <c r="C4" s="168" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="193"/>
+      <c r="D4" s="169"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="191"/>
-      <c r="G4" s="190"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="172"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="191" t="s">
+      <c r="C5" s="168" t="s">
         <v>212</v>
       </c>
-      <c r="D5" s="193"/>
+      <c r="D5" s="169"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="190"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="172"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="191" t="s">
+      <c r="C6" s="168" t="s">
         <v>213</v>
       </c>
-      <c r="D6" s="193"/>
+      <c r="D6" s="169"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="191"/>
-      <c r="G6" s="190"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="172"/>
     </row>
     <row r="7" spans="1:19" ht="13">
-      <c r="B7" s="175" t="s">
+      <c r="B7" s="177" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="177"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="178"/>
+      <c r="E7" s="178"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="179"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="178"/>
-      <c r="C8" s="179"/>
-      <c r="D8" s="179"/>
-      <c r="E8" s="179"/>
-      <c r="F8" s="179"/>
-      <c r="G8" s="180"/>
+      <c r="B8" s="180"/>
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="182"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="181"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
-      <c r="G9" s="180"/>
+      <c r="B9" s="183"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="182"/>
     </row>
     <row r="10" spans="1:19" ht="12" thickBot="1">
-      <c r="B10" s="182"/>
-      <c r="C10" s="183"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="184"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
+      <c r="F10" s="185"/>
+      <c r="G10" s="186"/>
     </row>
     <row r="12" spans="1:19" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10282,10 +10282,10 @@
       <c r="B27" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="185" t="s">
+      <c r="C27" s="187" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="186"/>
+      <c r="D27" s="188"/>
       <c r="E27" s="46" t="s">
         <v>3</v>
       </c>
@@ -10299,20 +10299,20 @@
         <v>2</v>
       </c>
       <c r="B28" s="51" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" s="192" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" s="193"/>
+      <c r="E28" s="52" t="s">
+        <v>239</v>
+      </c>
+      <c r="F28" s="52" t="s">
         <v>240</v>
       </c>
-      <c r="C28" s="171" t="s">
+      <c r="G28" s="53" t="s">
         <v>241</v>
-      </c>
-      <c r="D28" s="172"/>
-      <c r="E28" s="52" t="s">
-        <v>242</v>
-      </c>
-      <c r="F28" s="52" t="s">
-        <v>243</v>
-      </c>
-      <c r="G28" s="53" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="13" customHeight="1" thickBot="1">
@@ -10320,8 +10320,8 @@
         <v>3</v>
       </c>
       <c r="B29" s="54"/>
-      <c r="C29" s="169"/>
-      <c r="D29" s="170"/>
+      <c r="C29" s="190"/>
+      <c r="D29" s="191"/>
       <c r="E29" s="58"/>
       <c r="F29" s="58"/>
       <c r="G29" s="55"/>
@@ -10338,14 +10338,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="166" t="s">
+      <c r="C32" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="167"/>
-      <c r="E32" s="166" t="s">
+      <c r="D32" s="176"/>
+      <c r="E32" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="168"/>
+      <c r="F32" s="189"/>
       <c r="G32" s="38" t="s">
         <v>38</v>
       </c>
@@ -10355,10 +10355,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="19"/>
-      <c r="C33" s="185" t="s">
+      <c r="C33" s="187" t="s">
         <v>137</v>
       </c>
-      <c r="D33" s="186"/>
+      <c r="D33" s="188"/>
       <c r="E33" s="202" t="s">
         <v>151</v>
       </c>
@@ -10379,30 +10379,20 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="166" t="s">
+      <c r="C36" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="167"/>
-      <c r="E36" s="166" t="s">
+      <c r="D36" s="176"/>
+      <c r="E36" s="175" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="168"/>
+      <c r="F36" s="189"/>
       <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -10415,6 +10405,16 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10468,101 +10468,101 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="187" t="s">
+      <c r="C2" s="166" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="192"/>
+      <c r="D2" s="167"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="187"/>
-      <c r="G2" s="188"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="170"/>
     </row>
     <row r="3" spans="1:18" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="191"/>
-      <c r="D3" s="193"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="169"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="189" t="s">
+      <c r="F3" s="171" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="190"/>
+      <c r="G3" s="172"/>
     </row>
     <row r="4" spans="1:18" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="191" t="s">
+      <c r="C4" s="168" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="193"/>
+      <c r="D4" s="169"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="191"/>
-      <c r="G4" s="190"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="172"/>
     </row>
     <row r="5" spans="1:18" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="191" t="s">
+      <c r="C5" s="168" t="s">
         <v>222</v>
       </c>
-      <c r="D5" s="193"/>
+      <c r="D5" s="169"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="191"/>
-      <c r="G5" s="190"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="172"/>
     </row>
     <row r="6" spans="1:18" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="191" t="s">
+      <c r="C6" s="168" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="193"/>
+      <c r="D6" s="169"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="191"/>
-      <c r="G6" s="190"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="172"/>
     </row>
     <row r="7" spans="1:18" ht="13">
-      <c r="B7" s="175" t="s">
+      <c r="B7" s="177" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="177"/>
+      <c r="C7" s="178"/>
+      <c r="D7" s="178"/>
+      <c r="E7" s="178"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="179"/>
     </row>
     <row r="8" spans="1:18">
-      <c r="B8" s="178"/>
-      <c r="C8" s="179"/>
-      <c r="D8" s="179"/>
-      <c r="E8" s="179"/>
-      <c r="F8" s="179"/>
-      <c r="G8" s="180"/>
+      <c r="B8" s="180"/>
+      <c r="C8" s="181"/>
+      <c r="D8" s="181"/>
+      <c r="E8" s="181"/>
+      <c r="F8" s="181"/>
+      <c r="G8" s="182"/>
     </row>
     <row r="9" spans="1:18">
-      <c r="B9" s="181"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
-      <c r="G9" s="180"/>
+      <c r="B9" s="183"/>
+      <c r="C9" s="181"/>
+      <c r="D9" s="181"/>
+      <c r="E9" s="181"/>
+      <c r="F9" s="181"/>
+      <c r="G9" s="182"/>
     </row>
     <row r="10" spans="1:18" ht="12" thickBot="1">
-      <c r="B10" s="182"/>
-      <c r="C10" s="183"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="184"/>
+      <c r="B10" s="184"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="185"/>
+      <c r="F10" s="185"/>
+      <c r="G10" s="186"/>
     </row>
     <row r="12" spans="1:18" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10842,10 +10842,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="185" t="s">
+      <c r="C25" s="187" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="186"/>
+      <c r="D25" s="188"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -10859,8 +10859,8 @@
         <v>2</v>
       </c>
       <c r="B26" s="51"/>
-      <c r="C26" s="171"/>
-      <c r="D26" s="172"/>
+      <c r="C26" s="192"/>
+      <c r="D26" s="193"/>
       <c r="E26" s="46"/>
       <c r="F26" s="46"/>
       <c r="G26" s="20"/>
@@ -10870,8 +10870,8 @@
         <v>3</v>
       </c>
       <c r="B27" s="54"/>
-      <c r="C27" s="169"/>
-      <c r="D27" s="170"/>
+      <c r="C27" s="190"/>
+      <c r="D27" s="191"/>
       <c r="E27" s="58"/>
       <c r="F27" s="58"/>
       <c r="G27" s="55"/>
@@ -10888,14 +10888,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="166" t="s">
+      <c r="C30" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="167"/>
-      <c r="E30" s="166" t="s">
+      <c r="D30" s="176"/>
+      <c r="E30" s="175" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="168"/>
+      <c r="F30" s="189"/>
       <c r="G30" s="38" t="s">
         <v>38</v>
       </c>
@@ -10939,8 +10939,8 @@
         <v>3</v>
       </c>
       <c r="B33" s="54"/>
-      <c r="C33" s="169"/>
-      <c r="D33" s="170"/>
+      <c r="C33" s="190"/>
+      <c r="D33" s="191"/>
       <c r="E33" s="210"/>
       <c r="F33" s="211"/>
       <c r="G33" s="55"/>
@@ -10957,28 +10957,26 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="166" t="s">
+      <c r="C36" s="175" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="167"/>
-      <c r="E36" s="166" t="s">
+      <c r="D36" s="176"/>
+      <c r="E36" s="175" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="167"/>
+      <c r="F36" s="176"/>
       <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="F5:G5"/>
@@ -10991,12 +10989,14 @@
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>